<commit_message>
uh did it commit
</commit_message>
<xml_diff>
--- a/data/master_sheet.xlsx
+++ b/data/master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robot\Documents\NSS DA9\capstone_da9\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F94D227-10F0-42C9-9EBE-64EBA7508A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E296ED92-E9BA-4332-AAA1-A2D9A2F7C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4284" yWindow="3504" windowWidth="23040" windowHeight="12120" firstSheet="2" activeTab="6" xr2:uid="{3EC2733F-E7AB-4910-AA4F-3A2CDF5CDF4D}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="2" activeTab="2" xr2:uid="{3EC2733F-E7AB-4910-AA4F-3A2CDF5CDF4D}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="630">
   <si>
     <t>County</t>
   </si>
@@ -1892,6 +1892,57 @@
   </si>
   <si>
     <t>Hancock county has the lowest median income in TN</t>
+  </si>
+  <si>
+    <t>Amnicola Dump</t>
+  </si>
+  <si>
+    <t>Chemet Co.</t>
+  </si>
+  <si>
+    <t>Copper Basin Mining District</t>
+  </si>
+  <si>
+    <t>Copperhill</t>
+  </si>
+  <si>
+    <t>Gallaway Pits</t>
+  </si>
+  <si>
+    <t>ICG Iselin Railroad Yard</t>
+  </si>
+  <si>
+    <t>Illinois Central Railroad Company's Johnston Yard</t>
+  </si>
+  <si>
+    <t>Lewisburg Dump</t>
+  </si>
+  <si>
+    <t>North Hollywood Dump</t>
+  </si>
+  <si>
+    <t>Sixty One Industrial Park</t>
+  </si>
+  <si>
+    <t>Tennessee Products</t>
+  </si>
+  <si>
+    <t>Lewisburg</t>
+  </si>
+  <si>
+    <t>Somerville</t>
+  </si>
+  <si>
+    <t>superfunds</t>
+  </si>
+  <si>
+    <t>median_income</t>
+  </si>
+  <si>
+    <t>cancer_rates</t>
+  </si>
+  <si>
+    <t>Age-Adjusted incidence rate of cancer cases per 100,000</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +2031,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2023,6 +2074,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8310,10 +8364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7E8FA0-A0E0-4A69-AFEA-B0927D1B7F6E}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8327,9 +8381,12 @@
     <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>113</v>
       </c>
@@ -8369,8 +8426,17 @@
       <c r="M1" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -8410,8 +8476,17 @@
       <c r="M2" s="23">
         <v>147737</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" s="23">
+        <v>36286</v>
+      </c>
+      <c r="O2" s="9">
+        <v>3</v>
+      </c>
+      <c r="P2" s="9">
+        <v>512.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -8451,8 +8526,17 @@
       <c r="M3" s="24">
         <v>57889</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="24">
+        <v>26370</v>
+      </c>
+      <c r="O3" s="9">
+        <v>3</v>
+      </c>
+      <c r="P3" s="9">
+        <v>522.20000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -8492,8 +8576,17 @@
       <c r="M4" s="24">
         <v>158163</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" s="24">
+        <v>25192</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>510.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -8533,8 +8626,17 @@
       <c r="M5" s="24">
         <v>108620</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" s="24">
+        <v>26793</v>
+      </c>
+      <c r="O5" s="9">
+        <v>3</v>
+      </c>
+      <c r="P5" s="9">
+        <v>478.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -8574,8 +8676,17 @@
       <c r="M6" s="24">
         <v>341896</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" s="24">
+        <v>33593</v>
+      </c>
+      <c r="O6" s="9">
+        <v>6</v>
+      </c>
+      <c r="P6" s="9">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -8615,8 +8726,17 @@
       <c r="M7" s="24">
         <v>40953</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" s="24">
+        <v>24456</v>
+      </c>
+      <c r="O7" s="9">
+        <v>1</v>
+      </c>
+      <c r="P7" s="9">
+        <v>546.79999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -8656,8 +8776,17 @@
       <c r="M8" s="24">
         <v>196281</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" s="24">
+        <v>32861</v>
+      </c>
+      <c r="O8" s="9">
+        <v>3</v>
+      </c>
+      <c r="P8" s="9">
+        <v>516.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -8697,8 +8826,17 @@
       <c r="M9" s="24">
         <v>25143</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" s="24">
+        <v>24597</v>
+      </c>
+      <c r="O9" s="9">
+        <v>3</v>
+      </c>
+      <c r="P9" s="9">
+        <v>504.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -8738,8 +8876,17 @@
       <c r="M10" s="24">
         <v>135280</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10" s="24">
+        <v>30024</v>
+      </c>
+      <c r="O10" s="9">
+        <v>4</v>
+      </c>
+      <c r="P10" s="9">
+        <v>514.29999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -8779,8 +8926,17 @@
       <c r="M11" s="24">
         <v>53794</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11" s="24">
+        <v>24298</v>
+      </c>
+      <c r="O11" s="9">
+        <v>6</v>
+      </c>
+      <c r="P11" s="9">
+        <v>535.79999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -8820,8 +8976,17 @@
       <c r="M12" s="25">
         <v>6662</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" s="25">
+        <v>19165</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>578.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -8861,8 +9026,17 @@
       <c r="M13" s="25">
         <v>8283</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13" s="25">
+        <v>22684</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>620.79999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>13</v>
       </c>
@@ -8902,8 +9076,17 @@
       <c r="M14" s="25">
         <v>16232</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14" s="25">
+        <v>23219</v>
+      </c>
+      <c r="O14" s="8">
+        <v>3</v>
+      </c>
+      <c r="P14" s="8">
+        <v>494.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>14</v>
       </c>
@@ -8943,8 +9126,17 @@
       <c r="M15" s="25">
         <v>15864</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15" s="25">
+        <v>21145</v>
+      </c>
+      <c r="O15" s="8">
+        <v>4</v>
+      </c>
+      <c r="P15" s="8">
+        <v>576.70000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>15</v>
       </c>
@@ -8984,8 +9176,17 @@
       <c r="M16" s="25">
         <v>28837</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="25">
+        <v>24015</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>575.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -9025,8 +9226,17 @@
       <c r="M17" s="25">
         <v>7005</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="25">
+        <v>18397</v>
+      </c>
+      <c r="O17" s="8">
+        <v>1</v>
+      </c>
+      <c r="P17" s="8">
+        <v>479.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -9066,8 +9276,17 @@
       <c r="M18" s="25">
         <v>36801</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" s="25">
+        <v>26730</v>
+      </c>
+      <c r="O18" s="8">
+        <v>1</v>
+      </c>
+      <c r="P18" s="8">
+        <v>526.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -9107,8 +9326,17 @@
       <c r="M19" s="25">
         <v>32199</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19" s="25">
+        <v>25013</v>
+      </c>
+      <c r="O19" s="8">
+        <v>4</v>
+      </c>
+      <c r="P19" s="8">
+        <v>555.70000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -9148,8 +9376,17 @@
       <c r="M20" s="25">
         <v>13529</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20" s="25">
+        <v>21777</v>
+      </c>
+      <c r="O20" s="8">
+        <v>0</v>
+      </c>
+      <c r="P20" s="8">
+        <v>545.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>20</v>
       </c>
@@ -9189,8 +9426,20 @@
       <c r="M21" s="25">
         <v>18489</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21" s="25">
+        <v>19940</v>
+      </c>
+      <c r="O21" s="8">
+        <v>0</v>
+      </c>
+      <c r="P21" s="8">
+        <v>551.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="30">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>112</v>
       </c>
@@ -9223,6 +9472,12 @@
       </c>
       <c r="L22" s="14">
         <v>7.2</v>
+      </c>
+      <c r="N22" s="32">
+        <v>28995</v>
+      </c>
+      <c r="P22">
+        <v>514.70000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -9236,17 +9491,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CFF946-04A7-4B69-985C-4CC51394433A}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -9293,7 +9548,7 @@
         <v>0.13730000000000001</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D11" si="0">B3-C3</f>
+        <f t="shared" ref="D3:D15" si="0">B3-C3</f>
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="E3" s="7"/>
@@ -9434,6 +9689,71 @@
       <c r="D11" s="13">
         <f t="shared" si="0"/>
         <v>2.1000000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="31">
+        <f>AVERAGE('top and bottom 10'!M12:M21)</f>
+        <v>18390.099999999999</v>
+      </c>
+      <c r="C12" s="31">
+        <f>AVERAGE('top and bottom 10'!M2:M11)</f>
+        <v>126575.6</v>
+      </c>
+      <c r="D12" s="31">
+        <v>108186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>627</v>
+      </c>
+      <c r="B13" s="31">
+        <f>AVERAGE('top and bottom 10'!N12:N21)</f>
+        <v>22208.5</v>
+      </c>
+      <c r="C13" s="31">
+        <f>AVERAGE('top and bottom 10'!N2:N11)</f>
+        <v>28447</v>
+      </c>
+      <c r="D13" s="31">
+        <f>B13-C13</f>
+        <v>-6238.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>626</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>32</v>
+      </c>
+      <c r="D14" s="13">
+        <f t="shared" si="0"/>
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>628</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGE('top and bottom 10'!P12:P21)</f>
+        <v>550.5</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE('top and bottom 10'!P2:P11)</f>
+        <v>514.0200000000001</v>
+      </c>
+      <c r="D15" s="13">
+        <f t="shared" si="0"/>
+        <v>36.479999999999905</v>
       </c>
     </row>
   </sheetData>
@@ -9446,7 +9766,7 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9577,25 +9897,25 @@
     </row>
     <row r="2" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
-        <v>237</v>
+        <v>367</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>238</v>
+        <v>368</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>239</v>
+        <v>369</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>241</v>
+        <v>370</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>242</v>
+        <v>371</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>243</v>
@@ -9649,34 +9969,36 @@
       <c r="AA2" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB2" s="28"/>
+      <c r="AB2" s="28" t="s">
+        <v>372</v>
+      </c>
       <c r="AC2" s="29">
-        <v>40073</v>
+        <v>40177</v>
       </c>
       <c r="AD2" s="28"/>
       <c r="AE2" s="28"/>
     </row>
     <row r="3" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
-        <v>253</v>
+        <v>353</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>254</v>
+        <v>354</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>255</v>
+        <v>355</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>256</v>
+        <v>356</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>257</v>
+        <v>357</v>
       </c>
       <c r="H3" s="28" t="s">
         <v>243</v>
@@ -9719,7 +10041,7 @@
         <v>251</v>
       </c>
       <c r="V3" s="28" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="W3" s="28"/>
       <c r="X3" s="28" t="s">
@@ -9730,34 +10052,36 @@
       <c r="AA3" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB3" s="28"/>
+      <c r="AB3" s="28" t="s">
+        <v>358</v>
+      </c>
       <c r="AC3" s="29">
-        <v>42802</v>
+        <v>41240</v>
       </c>
       <c r="AD3" s="28"/>
       <c r="AE3" s="28"/>
     </row>
     <row r="4" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="H4" s="28" t="s">
         <v>243</v>
@@ -9788,20 +10112,16 @@
         <v>247</v>
       </c>
       <c r="R4" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S4" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T4" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U4" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>264</v>
-      </c>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
       <c r="W4" s="28"/>
       <c r="X4" s="28" t="s">
         <v>245</v>
@@ -9811,34 +10131,36 @@
       <c r="AA4" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB4" s="28"/>
+      <c r="AB4" s="28" t="s">
+        <v>269</v>
+      </c>
       <c r="AC4" s="29">
-        <v>43213</v>
+        <v>37351</v>
       </c>
       <c r="AD4" s="28"/>
       <c r="AE4" s="28"/>
     </row>
     <row r="5" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="E5" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="H5" s="28" t="s">
         <v>243</v>
@@ -9869,20 +10191,16 @@
         <v>247</v>
       </c>
       <c r="R5" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S5" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T5" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U5" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V5" s="28" t="s">
-        <v>252</v>
-      </c>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
       <c r="W5" s="28"/>
       <c r="X5" s="28" t="s">
         <v>245</v>
@@ -9894,32 +10212,32 @@
       </c>
       <c r="AB5" s="28"/>
       <c r="AC5" s="29">
-        <v>39336</v>
+        <v>37351</v>
       </c>
       <c r="AD5" s="28"/>
       <c r="AE5" s="28"/>
     </row>
     <row r="6" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
-        <v>268</v>
+        <v>432</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>269</v>
+        <v>433</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>270</v>
+        <v>434</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>271</v>
+        <v>435</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>272</v>
+        <v>436</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>243</v>
@@ -9947,58 +10265,58 @@
       </c>
       <c r="P6" s="28"/>
       <c r="Q6" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R6" s="28" t="s">
-        <v>273</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R6" s="28"/>
       <c r="S6" s="28" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="T6" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U6" s="28"/>
       <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
+      <c r="W6" s="28" t="s">
+        <v>437</v>
+      </c>
       <c r="X6" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y6" s="28"/>
       <c r="Z6" s="28"/>
       <c r="AA6" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="AB6" s="28" t="s">
-        <v>269</v>
+        <v>438</v>
       </c>
       <c r="AC6" s="29">
-        <v>37351</v>
+        <v>34806</v>
       </c>
       <c r="AD6" s="28"/>
       <c r="AE6" s="28"/>
     </row>
     <row r="7" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="28" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>270</v>
+        <v>291</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>272</v>
+        <v>293</v>
       </c>
       <c r="H7" s="28" t="s">
         <v>243</v>
@@ -10029,16 +10347,20 @@
         <v>247</v>
       </c>
       <c r="R7" s="28" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="S7" s="28" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="T7" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
+      <c r="U7" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="V7" s="28" t="s">
+        <v>264</v>
+      </c>
       <c r="W7" s="28"/>
       <c r="X7" s="28" t="s">
         <v>245</v>
@@ -10050,32 +10372,32 @@
       </c>
       <c r="AB7" s="28"/>
       <c r="AC7" s="29">
-        <v>37351</v>
+        <v>43280</v>
       </c>
       <c r="AD7" s="28"/>
       <c r="AE7" s="28"/>
     </row>
     <row r="8" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="28" t="s">
-        <v>278</v>
+        <v>373</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>279</v>
+        <v>374</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>280</v>
+        <v>375</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E8" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>281</v>
+        <v>376</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>282</v>
+        <v>377</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>243</v>
@@ -10103,22 +10425,20 @@
       </c>
       <c r="P8" s="28"/>
       <c r="Q8" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R8" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R8" s="28"/>
       <c r="S8" s="28" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="T8" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U8" s="28" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="V8" s="28" t="s">
-        <v>283</v>
+        <v>378</v>
       </c>
       <c r="W8" s="28"/>
       <c r="X8" s="28" t="s">
@@ -10129,34 +10449,36 @@
       <c r="AA8" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB8" s="28"/>
+      <c r="AB8" s="28" t="s">
+        <v>379</v>
+      </c>
       <c r="AC8" s="29">
-        <v>42191</v>
+        <v>39352</v>
       </c>
       <c r="AD8" s="28"/>
       <c r="AE8" s="28"/>
     </row>
     <row r="9" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
-        <v>284</v>
+        <v>487</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>285</v>
+        <v>488</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>270</v>
+        <v>489</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>286</v>
+        <v>490</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>287</v>
+        <v>491</v>
       </c>
       <c r="H9" s="28" t="s">
         <v>243</v>
@@ -10187,10 +10509,10 @@
         <v>247</v>
       </c>
       <c r="R9" s="28" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="S9" s="28" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="T9" s="28" t="s">
         <v>250</v>
@@ -10199,11 +10521,9 @@
         <v>251</v>
       </c>
       <c r="V9" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="W9" s="28" t="s">
-        <v>288</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="W9" s="28"/>
       <c r="X9" s="28" t="s">
         <v>245</v>
       </c>
@@ -10212,36 +10532,34 @@
       <c r="AA9" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB9" s="28" t="s">
-        <v>285</v>
-      </c>
+      <c r="AB9" s="28"/>
       <c r="AC9" s="29">
-        <v>31519</v>
+        <v>41199</v>
       </c>
       <c r="AD9" s="28"/>
       <c r="AE9" s="28"/>
     </row>
     <row r="10" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
-        <v>289</v>
+        <v>439</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>290</v>
+        <v>440</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>291</v>
+        <v>434</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="H10" s="28" t="s">
         <v>243</v>
@@ -10281,10 +10599,10 @@
         <v>250</v>
       </c>
       <c r="U10" s="28" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="V10" s="28" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="W10" s="28"/>
       <c r="X10" s="28" t="s">
@@ -10297,32 +10615,32 @@
       </c>
       <c r="AB10" s="28"/>
       <c r="AC10" s="29">
-        <v>43280</v>
+        <v>37937</v>
       </c>
       <c r="AD10" s="28"/>
       <c r="AE10" s="28"/>
     </row>
     <row r="11" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
-        <v>294</v>
+        <v>503</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>295</v>
+        <v>504</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>296</v>
+        <v>505</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>297</v>
+        <v>506</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>298</v>
+        <v>507</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>243</v>
@@ -10350,11 +10668,13 @@
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R11" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R11" s="28" t="s">
+        <v>248</v>
+      </c>
       <c r="S11" s="28" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="T11" s="28" t="s">
         <v>250</v>
@@ -10372,32 +10692,32 @@
       </c>
       <c r="AB11" s="28"/>
       <c r="AC11" s="29">
-        <v>37139</v>
+        <v>37354</v>
       </c>
       <c r="AD11" s="28"/>
       <c r="AE11" s="28"/>
     </row>
     <row r="12" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>296</v>
+        <v>329</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="H12" s="28" t="s">
         <v>243</v>
@@ -10428,20 +10748,16 @@
         <v>247</v>
       </c>
       <c r="R12" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S12" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T12" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U12" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V12" s="28" t="s">
-        <v>252</v>
-      </c>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
       <c r="W12" s="28"/>
       <c r="X12" s="28" t="s">
         <v>245</v>
@@ -10453,32 +10769,32 @@
       </c>
       <c r="AB12" s="28"/>
       <c r="AC12" s="29">
-        <v>38512</v>
+        <v>37238</v>
       </c>
       <c r="AD12" s="28"/>
       <c r="AE12" s="28"/>
     </row>
     <row r="13" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>243</v>
@@ -10517,8 +10833,12 @@
       <c r="T13" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
+      <c r="U13" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V13" s="28" t="s">
+        <v>283</v>
+      </c>
       <c r="W13" s="28"/>
       <c r="X13" s="28" t="s">
         <v>245</v>
@@ -10530,20 +10850,20 @@
       </c>
       <c r="AB13" s="28"/>
       <c r="AC13" s="29">
-        <v>37012</v>
+        <v>42191</v>
       </c>
       <c r="AD13" s="28"/>
       <c r="AE13" s="28"/>
     </row>
     <row r="14" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>66</v>
@@ -10552,10 +10872,10 @@
         <v>240</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>243</v>
@@ -10594,12 +10914,8 @@
       <c r="T14" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U14" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="V14" s="28" t="s">
-        <v>316</v>
-      </c>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
       <c r="W14" s="28"/>
       <c r="X14" s="28" t="s">
         <v>245</v>
@@ -10611,32 +10927,32 @@
       </c>
       <c r="AB14" s="28"/>
       <c r="AC14" s="29">
-        <v>41725</v>
+        <v>37012</v>
       </c>
       <c r="AD14" s="28"/>
       <c r="AE14" s="28"/>
     </row>
     <row r="15" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>317</v>
+        <v>380</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>318</v>
+        <v>381</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>312</v>
+        <v>375</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>319</v>
+        <v>382</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>304</v>
+        <v>377</v>
       </c>
       <c r="H15" s="28" t="s">
         <v>243</v>
@@ -10664,23 +10980,17 @@
       </c>
       <c r="P15" s="28"/>
       <c r="Q15" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R15" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R15" s="28"/>
       <c r="S15" s="28" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="T15" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U15" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V15" s="28" t="s">
-        <v>252</v>
-      </c>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
       <c r="W15" s="28"/>
       <c r="X15" s="28" t="s">
         <v>245</v>
@@ -10690,34 +11000,36 @@
       <c r="AA15" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB15" s="28"/>
+      <c r="AB15" s="28" t="s">
+        <v>383</v>
+      </c>
       <c r="AC15" s="29">
-        <v>39318</v>
+        <v>35025</v>
       </c>
       <c r="AD15" s="28"/>
       <c r="AE15" s="28"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>320</v>
+        <v>384</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>321</v>
+        <v>385</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>322</v>
+        <v>375</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>303</v>
+        <v>386</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>304</v>
+        <v>377</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>243</v>
@@ -10748,20 +11060,16 @@
         <v>323</v>
       </c>
       <c r="R16" s="28" t="s">
-        <v>324</v>
+        <v>387</v>
       </c>
       <c r="S16" s="28" t="s">
-        <v>325</v>
+        <v>388</v>
       </c>
       <c r="T16" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U16" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="V16" s="28" t="s">
-        <v>326</v>
-      </c>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
       <c r="W16" s="28"/>
       <c r="X16" s="28" t="s">
         <v>245</v>
@@ -10771,34 +11079,36 @@
       <c r="AA16" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB16" s="28"/>
+      <c r="AB16" s="28" t="s">
+        <v>385</v>
+      </c>
       <c r="AC16" s="29">
-        <v>41541</v>
+        <v>39051</v>
       </c>
       <c r="AD16" s="28"/>
       <c r="AE16" s="28"/>
     </row>
     <row r="17" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="H17" s="28" t="s">
         <v>243</v>
@@ -10850,32 +11160,32 @@
       </c>
       <c r="AB17" s="28"/>
       <c r="AC17" s="29">
-        <v>37238</v>
+        <v>37350</v>
       </c>
       <c r="AD17" s="28"/>
       <c r="AE17" s="28"/>
     </row>
     <row r="18" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>332</v>
+        <v>441</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>333</v>
+        <v>442</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>329</v>
+        <v>443</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E18" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="H18" s="28" t="s">
         <v>243</v>
@@ -10906,16 +11216,20 @@
         <v>247</v>
       </c>
       <c r="R18" s="28" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="T18" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
+      <c r="U18" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V18" s="28" t="s">
+        <v>252</v>
+      </c>
       <c r="W18" s="28"/>
       <c r="X18" s="28" t="s">
         <v>245</v>
@@ -10925,36 +11239,34 @@
       <c r="AA18" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB18" s="28" t="s">
-        <v>333</v>
-      </c>
+      <c r="AB18" s="28"/>
       <c r="AC18" s="29">
-        <v>36769</v>
+        <v>37175</v>
       </c>
       <c r="AD18" s="28"/>
       <c r="AE18" s="28"/>
     </row>
     <row r="19" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>335</v>
+        <v>444</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>336</v>
+        <v>445</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>337</v>
+        <v>443</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>338</v>
+        <v>446</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>339</v>
+        <v>447</v>
       </c>
       <c r="H19" s="28" t="s">
         <v>243</v>
@@ -10993,8 +11305,12 @@
       <c r="T19" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U19" s="28"/>
-      <c r="V19" s="28"/>
+      <c r="U19" s="28" t="s">
+        <v>263</v>
+      </c>
+      <c r="V19" s="28" t="s">
+        <v>264</v>
+      </c>
       <c r="W19" s="28"/>
       <c r="X19" s="28" t="s">
         <v>245</v>
@@ -11006,32 +11322,32 @@
       </c>
       <c r="AB19" s="28"/>
       <c r="AC19" s="29">
-        <v>37538</v>
+        <v>43014</v>
       </c>
       <c r="AD19" s="28"/>
       <c r="AE19" s="28"/>
     </row>
     <row r="20" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="28" t="s">
-        <v>340</v>
+        <v>468</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>341</v>
+        <v>469</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>337</v>
+        <v>470</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="E20" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>243</v>
@@ -11059,64 +11375,56 @@
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="28" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c r="R20" s="28" t="s">
-        <v>344</v>
+        <v>248</v>
       </c>
       <c r="S20" s="28" t="s">
-        <v>345</v>
+        <v>249</v>
       </c>
       <c r="T20" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U20" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V20" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="W20" s="28" t="s">
-        <v>346</v>
-      </c>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
       <c r="X20" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y20" s="28"/>
       <c r="Z20" s="28"/>
       <c r="AA20" s="28" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="AB20" s="28"/>
       <c r="AC20" s="29">
-        <v>42949</v>
+        <v>37354</v>
       </c>
       <c r="AD20" s="28"/>
-      <c r="AE20" s="28" t="s">
-        <v>348</v>
-      </c>
+      <c r="AE20" s="28"/>
     </row>
     <row r="21" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="28" t="s">
-        <v>349</v>
+        <v>448</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>350</v>
+        <v>449</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>351</v>
+        <v>443</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>303</v>
+        <v>450</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>352</v>
+        <v>451</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>243</v>
@@ -11144,13 +11452,11 @@
       </c>
       <c r="P21" s="28"/>
       <c r="Q21" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R21" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R21" s="28"/>
       <c r="S21" s="28" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="T21" s="28" t="s">
         <v>250</v>
@@ -11159,45 +11465,49 @@
         <v>251</v>
       </c>
       <c r="V21" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="W21" s="28"/>
+        <v>258</v>
+      </c>
+      <c r="W21" s="28" t="s">
+        <v>437</v>
+      </c>
       <c r="X21" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y21" s="28"/>
       <c r="Z21" s="28"/>
       <c r="AA21" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="AB21" s="28"/>
       <c r="AC21" s="29">
-        <v>42488</v>
+        <v>45167</v>
       </c>
       <c r="AD21" s="28"/>
-      <c r="AE21" s="28"/>
+      <c r="AE21" s="28" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="22" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="28" t="s">
-        <v>353</v>
+        <v>237</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>354</v>
+        <v>238</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>355</v>
+        <v>239</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>356</v>
+        <v>241</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>357</v>
+        <v>242</v>
       </c>
       <c r="H22" s="28" t="s">
         <v>243</v>
@@ -11251,36 +11561,34 @@
       <c r="AA22" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB22" s="28" t="s">
-        <v>358</v>
-      </c>
+      <c r="AB22" s="28"/>
       <c r="AC22" s="29">
-        <v>41240</v>
+        <v>40073</v>
       </c>
       <c r="AD22" s="28"/>
       <c r="AE22" s="28"/>
     </row>
     <row r="23" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
-        <v>359</v>
+        <v>481</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>360</v>
+        <v>482</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>361</v>
+        <v>483</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>362</v>
+        <v>484</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>304</v>
+        <v>485</v>
       </c>
       <c r="H23" s="28" t="s">
         <v>243</v>
@@ -11308,56 +11616,62 @@
       </c>
       <c r="P23" s="28"/>
       <c r="Q23" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R23" s="28" t="s">
-        <v>273</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R23" s="28"/>
       <c r="S23" s="28" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="T23" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U23" s="28"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="28"/>
+      <c r="U23" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V23" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="W23" s="28" t="s">
+        <v>437</v>
+      </c>
       <c r="X23" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y23" s="28"/>
       <c r="Z23" s="28"/>
       <c r="AA23" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="AB23" s="28"/>
       <c r="AC23" s="29">
-        <v>37350</v>
+        <v>45154</v>
       </c>
       <c r="AD23" s="28"/>
-      <c r="AE23" s="28"/>
+      <c r="AE23" s="28" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="24" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>363</v>
+        <v>403</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>364</v>
+        <v>404</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>361</v>
+        <v>405</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>55</v>
+        <v>406</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>365</v>
+        <v>407</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>366</v>
+        <v>408</v>
       </c>
       <c r="H24" s="28" t="s">
         <v>243</v>
@@ -11397,10 +11711,10 @@
         <v>250</v>
       </c>
       <c r="U24" s="28" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="V24" s="28" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="W24" s="28"/>
       <c r="X24" s="28" t="s">
@@ -11413,32 +11727,32 @@
       </c>
       <c r="AB24" s="28"/>
       <c r="AC24" s="29">
-        <v>39027</v>
+        <v>41959</v>
       </c>
       <c r="AD24" s="28"/>
       <c r="AE24" s="28"/>
     </row>
     <row r="25" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>367</v>
+        <v>453</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>368</v>
+        <v>454</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>369</v>
+        <v>455</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>370</v>
+        <v>456</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>371</v>
+        <v>457</v>
       </c>
       <c r="H25" s="28" t="s">
         <v>243</v>
@@ -11493,35 +11807,35 @@
         <v>245</v>
       </c>
       <c r="AB25" s="28" t="s">
-        <v>372</v>
+        <v>458</v>
       </c>
       <c r="AC25" s="29">
-        <v>40177</v>
+        <v>39940</v>
       </c>
       <c r="AD25" s="28"/>
       <c r="AE25" s="28"/>
     </row>
     <row r="26" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
-        <v>373</v>
+        <v>332</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>374</v>
+        <v>333</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>375</v>
+        <v>329</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>377</v>
+        <v>331</v>
       </c>
       <c r="H26" s="28" t="s">
         <v>243</v>
@@ -11549,21 +11863,19 @@
       </c>
       <c r="P26" s="28"/>
       <c r="Q26" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R26" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R26" s="28" t="s">
+        <v>273</v>
+      </c>
       <c r="S26" s="28" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="T26" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U26" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="V26" s="28" t="s">
-        <v>378</v>
-      </c>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
       <c r="W26" s="28"/>
       <c r="X26" s="28" t="s">
         <v>245</v>
@@ -11574,35 +11886,35 @@
         <v>245</v>
       </c>
       <c r="AB26" s="28" t="s">
-        <v>379</v>
+        <v>333</v>
       </c>
       <c r="AC26" s="29">
-        <v>39352</v>
+        <v>36769</v>
       </c>
       <c r="AD26" s="28"/>
       <c r="AE26" s="28"/>
     </row>
     <row r="27" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>375</v>
+        <v>397</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>243</v>
@@ -11639,8 +11951,12 @@
       <c r="T27" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U27" s="28"/>
-      <c r="V27" s="28"/>
+      <c r="U27" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="V27" s="28" t="s">
+        <v>401</v>
+      </c>
       <c r="W27" s="28"/>
       <c r="X27" s="28" t="s">
         <v>245</v>
@@ -11651,35 +11967,35 @@
         <v>245</v>
       </c>
       <c r="AB27" s="28" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
       <c r="AC27" s="29">
-        <v>35025</v>
+        <v>37355</v>
       </c>
       <c r="AD27" s="28"/>
       <c r="AE27" s="28"/>
     </row>
     <row r="28" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>384</v>
+        <v>294</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>385</v>
+        <v>295</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>375</v>
+        <v>296</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>386</v>
+        <v>297</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>377</v>
+        <v>298</v>
       </c>
       <c r="H28" s="28" t="s">
         <v>243</v>
@@ -11707,13 +12023,11 @@
       </c>
       <c r="P28" s="28"/>
       <c r="Q28" s="28" t="s">
-        <v>323</v>
-      </c>
-      <c r="R28" s="28" t="s">
-        <v>387</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R28" s="28"/>
       <c r="S28" s="28" t="s">
-        <v>388</v>
+        <v>300</v>
       </c>
       <c r="T28" s="28" t="s">
         <v>250</v>
@@ -11729,11 +12043,9 @@
       <c r="AA28" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB28" s="28" t="s">
-        <v>385</v>
-      </c>
+      <c r="AB28" s="28"/>
       <c r="AC28" s="29">
-        <v>39051</v>
+        <v>37139</v>
       </c>
       <c r="AD28" s="28"/>
       <c r="AE28" s="28"/>
@@ -11821,25 +12133,25 @@
     </row>
     <row r="30" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>392</v>
+        <v>253</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>393</v>
+        <v>254</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>375</v>
+        <v>255</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>394</v>
+        <v>256</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>377</v>
+        <v>257</v>
       </c>
       <c r="H30" s="28" t="s">
         <v>243</v>
@@ -11870,16 +12182,20 @@
         <v>247</v>
       </c>
       <c r="R30" s="28" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="S30" s="28" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="T30" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U30" s="28"/>
-      <c r="V30" s="28"/>
+      <c r="U30" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V30" s="28" t="s">
+        <v>258</v>
+      </c>
       <c r="W30" s="28"/>
       <c r="X30" s="28" t="s">
         <v>245</v>
@@ -11891,32 +12207,32 @@
       </c>
       <c r="AB30" s="28"/>
       <c r="AC30" s="29">
-        <v>36769</v>
+        <v>42802</v>
       </c>
       <c r="AD30" s="28"/>
       <c r="AE30" s="28"/>
     </row>
     <row r="31" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>395</v>
+        <v>310</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>396</v>
+        <v>311</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>397</v>
+        <v>312</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E31" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>398</v>
+        <v>313</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>399</v>
+        <v>314</v>
       </c>
       <c r="H31" s="28" t="s">
         <v>243</v>
@@ -11944,20 +12260,22 @@
       </c>
       <c r="P31" s="28"/>
       <c r="Q31" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R31" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R31" s="28" t="s">
+        <v>248</v>
+      </c>
       <c r="S31" s="28" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="T31" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U31" s="28" t="s">
-        <v>400</v>
+        <v>315</v>
       </c>
       <c r="V31" s="28" t="s">
-        <v>401</v>
+        <v>316</v>
       </c>
       <c r="W31" s="28"/>
       <c r="X31" s="28" t="s">
@@ -11968,36 +12286,34 @@
       <c r="AA31" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB31" s="28" t="s">
-        <v>402</v>
-      </c>
+      <c r="AB31" s="28"/>
       <c r="AC31" s="29">
-        <v>37355</v>
+        <v>41725</v>
       </c>
       <c r="AD31" s="28"/>
       <c r="AE31" s="28"/>
     </row>
     <row r="32" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>403</v>
+        <v>259</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>404</v>
+        <v>260</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>405</v>
+        <v>239</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>406</v>
+        <v>79</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>407</v>
+        <v>261</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>408</v>
+        <v>262</v>
       </c>
       <c r="H32" s="28" t="s">
         <v>243</v>
@@ -12040,7 +12356,7 @@
         <v>263</v>
       </c>
       <c r="V32" s="28" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="W32" s="28"/>
       <c r="X32" s="28" t="s">
@@ -12053,32 +12369,32 @@
       </c>
       <c r="AB32" s="28"/>
       <c r="AC32" s="29">
-        <v>41959</v>
+        <v>43213</v>
       </c>
       <c r="AD32" s="28"/>
       <c r="AE32" s="28"/>
     </row>
     <row r="33" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>409</v>
+        <v>265</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>410</v>
+        <v>266</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>411</v>
+        <v>239</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>406</v>
+        <v>79</v>
       </c>
       <c r="E33" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>412</v>
+        <v>267</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>413</v>
+        <v>242</v>
       </c>
       <c r="H33" s="28" t="s">
         <v>243</v>
@@ -12134,38 +12450,38 @@
       </c>
       <c r="AB33" s="28"/>
       <c r="AC33" s="29">
-        <v>42719</v>
+        <v>39336</v>
       </c>
       <c r="AD33" s="28"/>
       <c r="AE33" s="28"/>
     </row>
-    <row r="34" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>414</v>
+        <v>145</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>415</v>
+        <v>492</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>416</v>
+        <v>489</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>406</v>
+        <v>88</v>
       </c>
       <c r="E34" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>417</v>
+        <v>493</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>418</v>
+        <v>491</v>
       </c>
       <c r="H34" s="28" t="s">
         <v>243</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>244</v>
+        <v>494</v>
       </c>
       <c r="J34" s="28" t="s">
         <v>245</v>
@@ -12174,75 +12490,75 @@
         <v>245</v>
       </c>
       <c r="L34" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>246</v>
+        <v>347</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>246</v>
+        <v>347</v>
       </c>
       <c r="O34" s="28" t="s">
-        <v>245</v>
-      </c>
-      <c r="P34" s="28"/>
-      <c r="Q34" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R34" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="S34" s="28" t="s">
-        <v>249</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="P34" s="29">
+        <v>35332</v>
+      </c>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
       <c r="T34" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U34" s="28" t="s">
-        <v>400</v>
+        <v>263</v>
       </c>
       <c r="V34" s="28" t="s">
-        <v>401</v>
+        <v>495</v>
       </c>
       <c r="W34" s="28"/>
       <c r="X34" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y34" s="28"/>
-      <c r="Z34" s="28"/>
+      <c r="Z34" s="28">
+        <v>29.44</v>
+      </c>
       <c r="AA34" s="28" t="s">
         <v>245</v>
       </c>
       <c r="AB34" s="28" t="s">
-        <v>419</v>
+        <v>496</v>
       </c>
       <c r="AC34" s="29">
-        <v>37532</v>
-      </c>
-      <c r="AD34" s="28"/>
+        <v>29434</v>
+      </c>
+      <c r="AD34" s="28" t="s">
+        <v>497</v>
+      </c>
       <c r="AE34" s="28"/>
     </row>
     <row r="35" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>420</v>
+        <v>392</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>421</v>
+        <v>393</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>411</v>
+        <v>375</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>406</v>
+        <v>49</v>
       </c>
       <c r="E35" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>422</v>
+        <v>394</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>423</v>
+        <v>377</v>
       </c>
       <c r="H35" s="28" t="s">
         <v>243</v>
@@ -12294,17 +12610,17 @@
       </c>
       <c r="AB35" s="28"/>
       <c r="AC35" s="29">
-        <v>36740</v>
+        <v>36769</v>
       </c>
       <c r="AD35" s="28"/>
       <c r="AE35" s="28"/>
     </row>
     <row r="36" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>411</v>
@@ -12316,10 +12632,10 @@
         <v>240</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="H36" s="28" t="s">
         <v>243</v>
@@ -12347,62 +12663,60 @@
       </c>
       <c r="P36" s="28"/>
       <c r="Q36" s="28" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
       <c r="R36" s="28" t="s">
-        <v>344</v>
+        <v>248</v>
       </c>
       <c r="S36" s="28" t="s">
-        <v>345</v>
+        <v>249</v>
       </c>
       <c r="T36" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U36" s="28" t="s">
-        <v>400</v>
+        <v>251</v>
       </c>
       <c r="V36" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="W36" s="28" t="s">
-        <v>428</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="W36" s="28"/>
       <c r="X36" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y36" s="28"/>
       <c r="Z36" s="28"/>
       <c r="AA36" s="28" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="AB36" s="28"/>
       <c r="AC36" s="29">
-        <v>41305</v>
+        <v>42719</v>
       </c>
       <c r="AD36" s="28"/>
       <c r="AE36" s="28"/>
     </row>
     <row r="37" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>429</v>
+        <v>471</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>430</v>
+        <v>472</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>411</v>
+        <v>473</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>406</v>
+        <v>52</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>431</v>
+        <v>474</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>427</v>
+        <v>475</v>
       </c>
       <c r="H37" s="28" t="s">
         <v>243</v>
@@ -12430,23 +12744,17 @@
       </c>
       <c r="P37" s="28"/>
       <c r="Q37" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R37" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R37" s="28"/>
       <c r="S37" s="28" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="T37" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U37" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V37" s="28" t="s">
-        <v>252</v>
-      </c>
+      <c r="U37" s="28"/>
+      <c r="V37" s="28"/>
       <c r="W37" s="28"/>
       <c r="X37" s="28" t="s">
         <v>245</v>
@@ -12458,32 +12766,32 @@
       </c>
       <c r="AB37" s="28"/>
       <c r="AC37" s="29">
-        <v>43417</v>
+        <v>38230</v>
       </c>
       <c r="AD37" s="28"/>
       <c r="AE37" s="28"/>
     </row>
-    <row r="38" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="28" t="s">
-        <v>432</v>
+        <v>320</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>433</v>
+        <v>321</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>434</v>
+        <v>322</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>435</v>
+        <v>303</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>436</v>
+        <v>304</v>
       </c>
       <c r="H38" s="28" t="s">
         <v>243</v>
@@ -12511,58 +12819,60 @@
       </c>
       <c r="P38" s="28"/>
       <c r="Q38" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R38" s="28"/>
+        <v>323</v>
+      </c>
+      <c r="R38" s="28" t="s">
+        <v>324</v>
+      </c>
       <c r="S38" s="28" t="s">
-        <v>300</v>
+        <v>325</v>
       </c>
       <c r="T38" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28" t="s">
-        <v>437</v>
-      </c>
+      <c r="U38" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="V38" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="W38" s="28"/>
       <c r="X38" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y38" s="28"/>
       <c r="Z38" s="28"/>
       <c r="AA38" s="28" t="s">
-        <v>347</v>
-      </c>
-      <c r="AB38" s="28" t="s">
-        <v>438</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="AB38" s="28"/>
       <c r="AC38" s="29">
-        <v>34806</v>
+        <v>41541</v>
       </c>
       <c r="AD38" s="28"/>
       <c r="AE38" s="28"/>
     </row>
     <row r="39" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
-        <v>439</v>
+        <v>335</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>440</v>
+        <v>336</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>434</v>
+        <v>337</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="H39" s="28" t="s">
         <v>243</v>
@@ -12601,12 +12911,8 @@
       <c r="T39" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U39" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="V39" s="28" t="s">
-        <v>252</v>
-      </c>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
       <c r="W39" s="28"/>
       <c r="X39" s="28" t="s">
         <v>245</v>
@@ -12618,23 +12924,23 @@
       </c>
       <c r="AB39" s="28"/>
       <c r="AC39" s="29">
-        <v>37937</v>
+        <v>37538</v>
       </c>
       <c r="AD39" s="28"/>
       <c r="AE39" s="28"/>
     </row>
     <row r="40" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
-        <v>441</v>
+        <v>301</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>442</v>
+        <v>302</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>443</v>
+        <v>296</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>240</v>
@@ -12699,32 +13005,32 @@
       </c>
       <c r="AB40" s="28"/>
       <c r="AC40" s="29">
-        <v>37175</v>
+        <v>38512</v>
       </c>
       <c r="AD40" s="28"/>
       <c r="AE40" s="28"/>
     </row>
     <row r="41" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
-        <v>444</v>
+        <v>349</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>445</v>
+        <v>350</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>443</v>
+        <v>351</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>446</v>
+        <v>303</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>447</v>
+        <v>352</v>
       </c>
       <c r="H41" s="28" t="s">
         <v>243</v>
@@ -12764,10 +13070,10 @@
         <v>250</v>
       </c>
       <c r="U41" s="28" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="V41" s="28" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="W41" s="28"/>
       <c r="X41" s="28" t="s">
@@ -12780,32 +13086,32 @@
       </c>
       <c r="AB41" s="28"/>
       <c r="AC41" s="29">
-        <v>43014</v>
+        <v>42488</v>
       </c>
       <c r="AD41" s="28"/>
       <c r="AE41" s="28"/>
     </row>
     <row r="42" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
-        <v>448</v>
+        <v>476</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>449</v>
+        <v>477</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>443</v>
+        <v>478</v>
       </c>
       <c r="D42" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F42" s="28" t="s">
-        <v>450</v>
+        <v>479</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>451</v>
+        <v>480</v>
       </c>
       <c r="H42" s="28" t="s">
         <v>243</v>
@@ -12833,11 +13139,13 @@
       </c>
       <c r="P42" s="28"/>
       <c r="Q42" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R42" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R42" s="28" t="s">
+        <v>248</v>
+      </c>
       <c r="S42" s="28" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="T42" s="28" t="s">
         <v>250</v>
@@ -12846,49 +13154,45 @@
         <v>251</v>
       </c>
       <c r="V42" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="W42" s="28" t="s">
-        <v>437</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="W42" s="28"/>
       <c r="X42" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y42" s="28"/>
       <c r="Z42" s="28"/>
       <c r="AA42" s="28" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="AB42" s="28"/>
       <c r="AC42" s="29">
-        <v>45167</v>
+        <v>42907</v>
       </c>
       <c r="AD42" s="28"/>
-      <c r="AE42" s="28" t="s">
-        <v>452</v>
-      </c>
+      <c r="AE42" s="28"/>
     </row>
     <row r="43" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>453</v>
+        <v>414</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>454</v>
+        <v>415</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>455</v>
+        <v>416</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>61</v>
+        <v>406</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>456</v>
+        <v>417</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>457</v>
+        <v>418</v>
       </c>
       <c r="H43" s="28" t="s">
         <v>243</v>
@@ -12928,10 +13232,10 @@
         <v>250</v>
       </c>
       <c r="U43" s="28" t="s">
-        <v>251</v>
+        <v>400</v>
       </c>
       <c r="V43" s="28" t="s">
-        <v>252</v>
+        <v>401</v>
       </c>
       <c r="W43" s="28"/>
       <c r="X43" s="28" t="s">
@@ -12943,35 +13247,35 @@
         <v>245</v>
       </c>
       <c r="AB43" s="28" t="s">
-        <v>458</v>
+        <v>419</v>
       </c>
       <c r="AC43" s="29">
-        <v>39940</v>
+        <v>37532</v>
       </c>
       <c r="AD43" s="28"/>
       <c r="AE43" s="28"/>
     </row>
     <row r="44" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="28" t="s">
-        <v>459</v>
+        <v>420</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>460</v>
+        <v>421</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>61</v>
+        <v>406</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>461</v>
+        <v>422</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="H44" s="28" t="s">
         <v>243</v>
@@ -13002,20 +13306,16 @@
         <v>247</v>
       </c>
       <c r="R44" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S44" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T44" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U44" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="V44" s="28" t="s">
-        <v>462</v>
-      </c>
+      <c r="U44" s="28"/>
+      <c r="V44" s="28"/>
       <c r="W44" s="28"/>
       <c r="X44" s="28" t="s">
         <v>245</v>
@@ -13025,36 +13325,34 @@
       <c r="AA44" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB44" s="28" t="s">
-        <v>463</v>
-      </c>
+      <c r="AB44" s="28"/>
       <c r="AC44" s="29">
-        <v>37719</v>
+        <v>36740</v>
       </c>
       <c r="AD44" s="28"/>
       <c r="AE44" s="28"/>
     </row>
     <row r="45" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="28" t="s">
-        <v>464</v>
+        <v>508</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>465</v>
+        <v>509</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>443</v>
+        <v>505</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F45" s="28" t="s">
-        <v>466</v>
+        <v>510</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>467</v>
+        <v>507</v>
       </c>
       <c r="H45" s="28" t="s">
         <v>243</v>
@@ -13082,13 +13380,11 @@
       </c>
       <c r="P45" s="28"/>
       <c r="Q45" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="R45" s="28" t="s">
-        <v>248</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="R45" s="28"/>
       <c r="S45" s="28" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
       <c r="T45" s="28" t="s">
         <v>250</v>
@@ -13097,45 +13393,47 @@
         <v>251</v>
       </c>
       <c r="V45" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="W45" s="28"/>
+        <v>258</v>
+      </c>
+      <c r="W45" s="28" t="s">
+        <v>437</v>
+      </c>
       <c r="X45" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y45" s="28"/>
       <c r="Z45" s="28"/>
       <c r="AA45" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="AB45" s="28"/>
       <c r="AC45" s="29">
-        <v>39358</v>
+        <v>44620</v>
       </c>
       <c r="AD45" s="28"/>
       <c r="AE45" s="28"/>
     </row>
     <row r="46" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="28" t="s">
-        <v>468</v>
+        <v>340</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>469</v>
+        <v>341</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>470</v>
+        <v>337</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>304</v>
+        <v>343</v>
       </c>
       <c r="H46" s="28" t="s">
         <v>243</v>
@@ -13163,56 +13461,64 @@
       </c>
       <c r="P46" s="28"/>
       <c r="Q46" s="28" t="s">
-        <v>247</v>
+        <v>323</v>
       </c>
       <c r="R46" s="28" t="s">
-        <v>248</v>
+        <v>344</v>
       </c>
       <c r="S46" s="28" t="s">
-        <v>249</v>
+        <v>345</v>
       </c>
       <c r="T46" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U46" s="28"/>
-      <c r="V46" s="28"/>
-      <c r="W46" s="28"/>
+      <c r="U46" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V46" s="28" t="s">
+        <v>258</v>
+      </c>
+      <c r="W46" s="28" t="s">
+        <v>346</v>
+      </c>
       <c r="X46" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y46" s="28"/>
       <c r="Z46" s="28"/>
       <c r="AA46" s="28" t="s">
-        <v>245</v>
+        <v>347</v>
       </c>
       <c r="AB46" s="28"/>
       <c r="AC46" s="29">
-        <v>37354</v>
+        <v>42949</v>
       </c>
       <c r="AD46" s="28"/>
-      <c r="AE46" s="28"/>
+      <c r="AE46" s="28" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="47" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="28" t="s">
-        <v>471</v>
+        <v>363</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>472</v>
+        <v>364</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>473</v>
+        <v>361</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>474</v>
+        <v>365</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>475</v>
+        <v>366</v>
       </c>
       <c r="H47" s="28" t="s">
         <v>243</v>
@@ -13240,17 +13546,23 @@
       </c>
       <c r="P47" s="28"/>
       <c r="Q47" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R47" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R47" s="28" t="s">
+        <v>248</v>
+      </c>
       <c r="S47" s="28" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="T47" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U47" s="28"/>
-      <c r="V47" s="28"/>
+      <c r="U47" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="V47" s="28" t="s">
+        <v>252</v>
+      </c>
       <c r="W47" s="28"/>
       <c r="X47" s="28" t="s">
         <v>245</v>
@@ -13262,32 +13574,32 @@
       </c>
       <c r="AB47" s="28"/>
       <c r="AC47" s="29">
-        <v>38230</v>
+        <v>39027</v>
       </c>
       <c r="AD47" s="28"/>
       <c r="AE47" s="28"/>
     </row>
     <row r="48" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="28" t="s">
-        <v>476</v>
+        <v>284</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>477</v>
+        <v>285</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>478</v>
+        <v>270</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E48" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>479</v>
+        <v>286</v>
       </c>
       <c r="G48" s="28" t="s">
-        <v>480</v>
+        <v>287</v>
       </c>
       <c r="H48" s="28" t="s">
         <v>243</v>
@@ -13318,10 +13630,10 @@
         <v>247</v>
       </c>
       <c r="R48" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S48" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T48" s="28" t="s">
         <v>250</v>
@@ -13330,9 +13642,11 @@
         <v>251</v>
       </c>
       <c r="V48" s="28" t="s">
-        <v>283</v>
-      </c>
-      <c r="W48" s="28"/>
+        <v>258</v>
+      </c>
+      <c r="W48" s="28" t="s">
+        <v>288</v>
+      </c>
       <c r="X48" s="28" t="s">
         <v>245</v>
       </c>
@@ -13341,34 +13655,36 @@
       <c r="AA48" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB48" s="28"/>
+      <c r="AB48" s="28" t="s">
+        <v>285</v>
+      </c>
       <c r="AC48" s="29">
-        <v>42907</v>
+        <v>31519</v>
       </c>
       <c r="AD48" s="28"/>
       <c r="AE48" s="28"/>
     </row>
     <row r="49" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="28" t="s">
-        <v>481</v>
+        <v>424</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>482</v>
+        <v>425</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>483</v>
+        <v>411</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>86</v>
+        <v>406</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>484</v>
+        <v>426</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>485</v>
+        <v>427</v>
       </c>
       <c r="H49" s="28" t="s">
         <v>243</v>
@@ -13396,23 +13712,25 @@
       </c>
       <c r="P49" s="28"/>
       <c r="Q49" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R49" s="28"/>
+        <v>323</v>
+      </c>
+      <c r="R49" s="28" t="s">
+        <v>344</v>
+      </c>
       <c r="S49" s="28" t="s">
-        <v>300</v>
+        <v>345</v>
       </c>
       <c r="T49" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U49" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="V49" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="V49" s="28" t="s">
-        <v>258</v>
-      </c>
       <c r="W49" s="28" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="X49" s="28" t="s">
         <v>245</v>
@@ -13424,34 +13742,32 @@
       </c>
       <c r="AB49" s="28"/>
       <c r="AC49" s="29">
-        <v>45154</v>
+        <v>41305</v>
       </c>
       <c r="AD49" s="28"/>
-      <c r="AE49" s="28" t="s">
-        <v>486</v>
-      </c>
+      <c r="AE49" s="28"/>
     </row>
     <row r="50" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="28" t="s">
-        <v>487</v>
+        <v>459</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>488</v>
+        <v>460</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>489</v>
+        <v>434</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F50" s="28" t="s">
-        <v>490</v>
+        <v>461</v>
       </c>
       <c r="G50" s="28" t="s">
-        <v>491</v>
+        <v>436</v>
       </c>
       <c r="H50" s="28" t="s">
         <v>243</v>
@@ -13491,10 +13807,10 @@
         <v>250</v>
       </c>
       <c r="U50" s="28" t="s">
-        <v>251</v>
+        <v>315</v>
       </c>
       <c r="V50" s="28" t="s">
-        <v>252</v>
+        <v>462</v>
       </c>
       <c r="W50" s="28"/>
       <c r="X50" s="28" t="s">
@@ -13505,40 +13821,42 @@
       <c r="AA50" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB50" s="28"/>
+      <c r="AB50" s="28" t="s">
+        <v>463</v>
+      </c>
       <c r="AC50" s="29">
-        <v>41199</v>
+        <v>37719</v>
       </c>
       <c r="AD50" s="28"/>
       <c r="AE50" s="28"/>
     </row>
-    <row r="51" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="28" t="s">
-        <v>145</v>
+        <v>317</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>492</v>
+        <v>318</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>489</v>
+        <v>312</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E51" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F51" s="28" t="s">
-        <v>493</v>
+        <v>319</v>
       </c>
       <c r="G51" s="28" t="s">
-        <v>491</v>
+        <v>304</v>
       </c>
       <c r="H51" s="28" t="s">
         <v>243</v>
       </c>
       <c r="I51" s="28" t="s">
-        <v>494</v>
+        <v>244</v>
       </c>
       <c r="J51" s="28" t="s">
         <v>245</v>
@@ -13547,75 +13865,73 @@
         <v>245</v>
       </c>
       <c r="L51" s="28" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="M51" s="28" t="s">
-        <v>347</v>
+        <v>246</v>
       </c>
       <c r="N51" s="28" t="s">
-        <v>347</v>
+        <v>246</v>
       </c>
       <c r="O51" s="28" t="s">
-        <v>347</v>
-      </c>
-      <c r="P51" s="29">
-        <v>35332</v>
-      </c>
-      <c r="Q51" s="28"/>
-      <c r="R51" s="28"/>
-      <c r="S51" s="28"/>
+        <v>245</v>
+      </c>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="R51" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="S51" s="28" t="s">
+        <v>249</v>
+      </c>
       <c r="T51" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U51" s="28" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="V51" s="28" t="s">
-        <v>495</v>
+        <v>252</v>
       </c>
       <c r="W51" s="28"/>
       <c r="X51" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y51" s="28"/>
-      <c r="Z51" s="28">
-        <v>29.44</v>
-      </c>
+      <c r="Z51" s="28"/>
       <c r="AA51" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB51" s="28" t="s">
-        <v>496</v>
-      </c>
+      <c r="AB51" s="28"/>
       <c r="AC51" s="29">
-        <v>29434</v>
-      </c>
-      <c r="AD51" s="28" t="s">
-        <v>497</v>
-      </c>
+        <v>39318</v>
+      </c>
+      <c r="AD51" s="28"/>
       <c r="AE51" s="28"/>
     </row>
     <row r="52" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="28" t="s">
-        <v>498</v>
+        <v>429</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>499</v>
+        <v>430</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>489</v>
+        <v>411</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>88</v>
+        <v>406</v>
       </c>
       <c r="E52" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>500</v>
+        <v>431</v>
       </c>
       <c r="G52" s="28" t="s">
-        <v>491</v>
+        <v>427</v>
       </c>
       <c r="H52" s="28" t="s">
         <v>243</v>
@@ -13646,19 +13962,19 @@
         <v>247</v>
       </c>
       <c r="R52" s="28" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="S52" s="28" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="T52" s="28" t="s">
         <v>250</v>
       </c>
       <c r="U52" s="28" t="s">
-        <v>400</v>
+        <v>251</v>
       </c>
       <c r="V52" s="28" t="s">
-        <v>501</v>
+        <v>252</v>
       </c>
       <c r="W52" s="28"/>
       <c r="X52" s="28" t="s">
@@ -13669,36 +13985,34 @@
       <c r="AA52" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB52" s="28" t="s">
-        <v>502</v>
-      </c>
+      <c r="AB52" s="28"/>
       <c r="AC52" s="29">
-        <v>33910</v>
+        <v>43417</v>
       </c>
       <c r="AD52" s="28"/>
       <c r="AE52" s="28"/>
     </row>
     <row r="53" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="28" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E53" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="H53" s="28" t="s">
         <v>243</v>
@@ -13729,16 +14043,20 @@
         <v>247</v>
       </c>
       <c r="R53" s="28" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="S53" s="28" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="T53" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="U53" s="28"/>
-      <c r="V53" s="28"/>
+      <c r="U53" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="V53" s="28" t="s">
+        <v>501</v>
+      </c>
       <c r="W53" s="28"/>
       <c r="X53" s="28" t="s">
         <v>245</v>
@@ -13748,34 +14066,36 @@
       <c r="AA53" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="AB53" s="28"/>
+      <c r="AB53" s="28" t="s">
+        <v>502</v>
+      </c>
       <c r="AC53" s="29">
-        <v>37354</v>
+        <v>33910</v>
       </c>
       <c r="AD53" s="28"/>
       <c r="AE53" s="28"/>
     </row>
     <row r="54" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="28" t="s">
-        <v>508</v>
+        <v>464</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>509</v>
+        <v>465</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>505</v>
+        <v>443</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E54" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F54" s="28" t="s">
-        <v>510</v>
+        <v>466</v>
       </c>
       <c r="G54" s="28" t="s">
-        <v>507</v>
+        <v>467</v>
       </c>
       <c r="H54" s="28" t="s">
         <v>243</v>
@@ -13803,11 +14123,13 @@
       </c>
       <c r="P54" s="28"/>
       <c r="Q54" s="28" t="s">
-        <v>299</v>
-      </c>
-      <c r="R54" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="R54" s="28" t="s">
+        <v>248</v>
+      </c>
       <c r="S54" s="28" t="s">
-        <v>300</v>
+        <v>249</v>
       </c>
       <c r="T54" s="28" t="s">
         <v>250</v>
@@ -13816,22 +14138,20 @@
         <v>251</v>
       </c>
       <c r="V54" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="W54" s="28" t="s">
-        <v>437</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="W54" s="28"/>
       <c r="X54" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Y54" s="28"/>
       <c r="Z54" s="28"/>
       <c r="AA54" s="28" t="s">
-        <v>347</v>
+        <v>245</v>
       </c>
       <c r="AB54" s="28"/>
       <c r="AC54" s="29">
-        <v>44620</v>
+        <v>39358</v>
       </c>
       <c r="AD54" s="28"/>
       <c r="AE54" s="28"/>
@@ -13918,26 +14238,32 @@
       <c r="AE55" s="28"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE55">
+    <sortCondition ref="B1:B55"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64026CDF-F6F6-486A-BF3A-E90CD57FEDD7}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
@@ -13945,16 +14271,22 @@
         <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -13962,16 +14294,22 @@
         <v>126</v>
       </c>
       <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
+        <v>534</v>
+      </c>
+      <c r="E2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="26">
+      <c r="F2" s="26">
         <v>40802</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -13979,307 +14317,565 @@
         <v>129</v>
       </c>
       <c r="C3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" t="s">
+        <v>582</v>
+      </c>
+      <c r="E3" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="26">
+      <c r="F3" s="26">
         <v>31573</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>35.22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>613</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F4" s="26"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>132</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" t="s">
+        <v>551</v>
+      </c>
+      <c r="E5" t="s">
         <v>133</v>
       </c>
-      <c r="D4" s="26">
+      <c r="F5" s="26">
         <v>31980</v>
       </c>
-      <c r="E4">
+      <c r="G5">
         <v>39.03</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>135</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="26">
+      <c r="F6" s="26">
         <v>32925</v>
       </c>
-      <c r="E5">
+      <c r="G6">
         <v>48.91</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B7" t="s">
+        <v>625</v>
+      </c>
+      <c r="C7" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" t="s">
+        <v>576</v>
+      </c>
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>137</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>138</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" t="s">
+        <v>580</v>
+      </c>
+      <c r="E8" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="26">
+      <c r="F8" s="26">
         <v>41418</v>
       </c>
-      <c r="E6">
+      <c r="G8">
         <v>48.03</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>615</v>
+      </c>
+      <c r="B9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>564</v>
+      </c>
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>140</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10" t="s">
+        <v>551</v>
+      </c>
+      <c r="E10" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="26">
+      <c r="F10" s="26">
         <v>42950</v>
       </c>
-      <c r="E7">
+      <c r="G10">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>617</v>
+      </c>
+      <c r="B11" t="s">
+        <v>576</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>576</v>
+      </c>
+      <c r="F11" s="26"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>618</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" t="s">
+        <v>582</v>
+      </c>
+      <c r="F12" s="26"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>619</v>
+      </c>
+      <c r="B13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" t="s">
+        <v>551</v>
+      </c>
+      <c r="F13" s="26"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>620</v>
+      </c>
+      <c r="B14" t="s">
+        <v>624</v>
+      </c>
+      <c r="C14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" t="s">
+        <v>538</v>
+      </c>
+      <c r="F14" s="26"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>143</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B15" t="s">
         <v>144</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>518</v>
+      </c>
+      <c r="E15" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="26">
+      <c r="F15" s="26">
         <v>32785</v>
       </c>
-      <c r="E8">
+      <c r="G15">
         <v>29.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>146</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B16" t="s">
         <v>141</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C16" t="s">
+        <v>240</v>
+      </c>
+      <c r="D16" t="s">
+        <v>551</v>
+      </c>
+      <c r="E16" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="26">
+      <c r="F16" s="26">
         <v>33891</v>
       </c>
-      <c r="E9">
+      <c r="G16">
         <v>58.06</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>148</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B17" t="s">
         <v>149</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" t="s">
+        <v>563</v>
+      </c>
+      <c r="E17" t="s">
         <v>150</v>
       </c>
-      <c r="D10" s="26">
+      <c r="F17" s="26">
         <v>31980</v>
       </c>
-      <c r="E10">
+      <c r="G17">
         <v>58.15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>151</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B18" t="s">
         <v>152</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D18" t="s">
+        <v>527</v>
+      </c>
+      <c r="E18" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="26">
+      <c r="F18" s="26">
         <v>30567</v>
       </c>
-      <c r="E11">
+      <c r="G18">
         <v>46.44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>154</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B19" t="s">
         <v>155</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C19" t="s">
+        <v>240</v>
+      </c>
+      <c r="D19" t="s">
+        <v>551</v>
+      </c>
+      <c r="E19" t="s">
         <v>156</v>
       </c>
-      <c r="D12" s="26">
+      <c r="F19" s="26">
         <v>44636</v>
       </c>
-      <c r="E12">
+      <c r="G19">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>621</v>
+      </c>
+      <c r="B20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" t="s">
+        <v>551</v>
+      </c>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>157</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B21" t="s">
         <v>158</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C21" t="s">
+        <v>240</v>
+      </c>
+      <c r="D21" t="s">
+        <v>579</v>
+      </c>
+      <c r="E21" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="26">
+      <c r="F21" s="26">
         <v>32833</v>
       </c>
-      <c r="E13">
+      <c r="G21">
         <v>51.13</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>160</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B22" t="s">
         <v>161</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C22" t="s">
+        <v>240</v>
+      </c>
+      <c r="D22" t="s">
+        <v>576</v>
+      </c>
+      <c r="E22" t="s">
         <v>162</v>
       </c>
-      <c r="D14" s="26">
+      <c r="F22" s="26">
         <v>35521</v>
       </c>
-      <c r="E14">
+      <c r="G22">
         <v>37.65</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>622</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" t="s">
+        <v>240</v>
+      </c>
+      <c r="D23" t="s">
+        <v>551</v>
+      </c>
+      <c r="F23" s="26"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>163</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B24" t="s">
         <v>135</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D24" t="s">
+        <v>551</v>
+      </c>
+      <c r="E24" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="26">
+      <c r="F24" s="26">
         <v>38469</v>
       </c>
-      <c r="E15">
+      <c r="G24">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>165</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B25" t="s">
         <v>166</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C25" t="s">
+        <v>240</v>
+      </c>
+      <c r="D25" t="s">
+        <v>584</v>
+      </c>
+      <c r="E25" t="s">
         <v>167</v>
       </c>
-      <c r="D16" s="26">
+      <c r="F25" s="26">
         <v>40450</v>
       </c>
-      <c r="E16">
+      <c r="G25">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>168</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B26" t="s">
         <v>169</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C26" t="s">
+        <v>240</v>
+      </c>
+      <c r="D26" t="s">
+        <v>565</v>
+      </c>
+      <c r="E26" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="26">
+      <c r="F26" s="26">
         <v>43356</v>
       </c>
-      <c r="E17">
+      <c r="G26">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>623</v>
+      </c>
+      <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>240</v>
+      </c>
+      <c r="D27" t="s">
+        <v>565</v>
+      </c>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>171</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B28" t="s">
         <v>172</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" t="s">
+        <v>559</v>
+      </c>
+      <c r="E28" t="s">
         <v>173</v>
       </c>
-      <c r="D18" s="26">
+      <c r="F28" s="26">
         <v>30567</v>
       </c>
-      <c r="E18">
+      <c r="G28">
         <v>47.71</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>174</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B29" t="s">
         <v>135</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C29" t="s">
+        <v>240</v>
+      </c>
+      <c r="D29" t="s">
+        <v>551</v>
+      </c>
+      <c r="E29" t="s">
         <v>175</v>
       </c>
-      <c r="D19" s="26">
+      <c r="F29" s="26">
         <v>41771</v>
       </c>
-      <c r="E19">
+      <c r="G29">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>176</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>177</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C30" t="s">
+        <v>240</v>
+      </c>
+      <c r="D30" t="s">
+        <v>536</v>
+      </c>
+      <c r="E30" t="s">
         <v>178</v>
       </c>
-      <c r="D20" s="26">
+      <c r="F30" s="26">
         <v>32598</v>
       </c>
-      <c r="E20">
+      <c r="G30">
         <v>36.14</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E79">
-    <sortCondition ref="A2:A79"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G30">
+    <sortCondition ref="A1:A30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14289,8 +14885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A65B623-EEE1-40F2-BEEC-3DE3D8C2404B}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14378,6 +14974,14 @@
       </c>
       <c r="C10" t="s">
         <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>628</v>
+      </c>
+      <c r="C11" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>